<commit_message>
Sign In test scripts finished.
</commit_message>
<xml_diff>
--- a/Test Plan/Test Cases - in progress.xlsx
+++ b/Test Plan/Test Cases - in progress.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="372">
   <si>
     <t>Project Name (Client Name)</t>
   </si>
@@ -800,9 +800,6 @@
     <t>TC_LF_010</t>
   </si>
   <si>
-    <t>IN PROGRESS</t>
-  </si>
-  <si>
     <t>Validate Loggingout from the Application and browsing back using Browser back button</t>
   </si>
   <si>
@@ -827,7 +824,7 @@
     <t>TC_LF_012</t>
   </si>
   <si>
-    <t>Validate the text into the Password field is toggled to hide its visibility</t>
+    <t xml:space="preserve">Validate the text into the Password field is toggled to hide its visibility. Check if Password is masked with dots. </t>
   </si>
   <si>
     <t xml:space="preserve">1.Click on ‘Sign In’ on top home page menu(Validate ER-1)
@@ -3695,22 +3692,22 @@
         <v>137</v>
       </c>
       <c r="C12" s="48" t="s">
+        <v>163</v>
+      </c>
+      <c r="D12" s="41" t="s">
         <v>175</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>176</v>
       </c>
       <c r="E12" s="38" t="s">
         <v>51</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G12" s="32" t="s">
         <v>141</v>
       </c>
       <c r="H12" s="38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="I12" s="43"/>
       <c r="J12" s="43"/>
@@ -3719,7 +3716,7 @@
     </row>
     <row r="13" ht="18.0" customHeight="1">
       <c r="A13" s="50" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B13" s="51" t="s">
         <v>137</v>
@@ -3728,7 +3725,7 @@
         <v>163</v>
       </c>
       <c r="D13" s="53" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="E13" s="54" t="s">
         <v>51</v>
@@ -3745,28 +3742,28 @@
     </row>
     <row r="14" ht="18.0" customHeight="1">
       <c r="A14" s="30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B14" s="37" t="s">
         <v>137</v>
       </c>
       <c r="C14" s="48" t="s">
-        <v>175</v>
-      </c>
-      <c r="D14" s="41" t="s">
-        <v>182</v>
+        <v>163</v>
+      </c>
+      <c r="D14" s="38" t="s">
+        <v>181</v>
       </c>
       <c r="E14" s="38" t="s">
         <v>51</v>
       </c>
       <c r="F14" s="32" t="s">
+        <v>182</v>
+      </c>
+      <c r="G14" s="32" t="s">
         <v>183</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="H14" s="38" t="s">
         <v>184</v>
-      </c>
-      <c r="H14" s="38" t="s">
-        <v>185</v>
       </c>
       <c r="I14" s="43"/>
       <c r="J14" s="43"/>
@@ -3775,28 +3772,28 @@
     </row>
     <row r="15" ht="18.0" customHeight="1">
       <c r="A15" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B15" s="37" t="s">
         <v>137</v>
       </c>
       <c r="C15" s="48" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E15" s="38" t="s">
         <v>51</v>
       </c>
       <c r="F15" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H15" s="38" t="s">
         <v>188</v>
-      </c>
-      <c r="G15" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="38" t="s">
-        <v>189</v>
       </c>
       <c r="I15" s="43"/>
       <c r="J15" s="43"/>
@@ -3805,7 +3802,7 @@
     </row>
     <row r="16" ht="18.0" customHeight="1">
       <c r="A16" s="50" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B16" s="58" t="s">
         <v>137</v>
@@ -3814,19 +3811,19 @@
         <v>163</v>
       </c>
       <c r="D16" s="59" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E16" s="60" t="s">
         <v>51</v>
       </c>
       <c r="F16" s="54" t="s">
+        <v>191</v>
+      </c>
+      <c r="G16" s="54" t="s">
         <v>192</v>
       </c>
-      <c r="G16" s="54" t="s">
+      <c r="H16" s="59" t="s">
         <v>193</v>
-      </c>
-      <c r="H16" s="59" t="s">
-        <v>194</v>
       </c>
       <c r="I16" s="61"/>
       <c r="J16" s="61"/>
@@ -3835,7 +3832,7 @@
     </row>
     <row r="17" ht="18.0" customHeight="1">
       <c r="A17" s="50" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B17" s="58" t="s">
         <v>137</v>
@@ -3844,19 +3841,19 @@
         <v>163</v>
       </c>
       <c r="D17" s="63" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E17" s="60" t="s">
         <v>51</v>
       </c>
       <c r="F17" s="64" t="s">
+        <v>196</v>
+      </c>
+      <c r="G17" s="65" t="s">
         <v>197</v>
       </c>
-      <c r="G17" s="65" t="s">
+      <c r="H17" s="60" t="s">
         <v>198</v>
-      </c>
-      <c r="H17" s="60" t="s">
-        <v>199</v>
       </c>
       <c r="I17" s="61"/>
       <c r="J17" s="61"/>
@@ -3865,26 +3862,26 @@
     </row>
     <row r="18" ht="18.0" customHeight="1">
       <c r="A18" s="30" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>137</v>
       </c>
       <c r="C18" s="48" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E18" s="38" t="s">
         <v>51</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G18" s="30"/>
       <c r="H18" s="38" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="I18" s="43"/>
       <c r="J18" s="43"/>
@@ -3893,7 +3890,7 @@
     </row>
     <row r="19" ht="18.0" customHeight="1">
       <c r="A19" s="50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B19" s="58" t="s">
         <v>137</v>
@@ -3902,19 +3899,19 @@
         <v>163</v>
       </c>
       <c r="D19" s="59" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E19" s="60" t="s">
         <v>51</v>
       </c>
       <c r="F19" s="54" t="s">
+        <v>205</v>
+      </c>
+      <c r="G19" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="H19" s="59" t="s">
         <v>206</v>
-      </c>
-      <c r="G19" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="H19" s="59" t="s">
-        <v>207</v>
       </c>
       <c r="I19" s="61"/>
       <c r="J19" s="61"/>
@@ -3923,16 +3920,16 @@
     </row>
     <row r="20" ht="18.0" customHeight="1">
       <c r="A20" s="30" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B20" s="37" t="s">
         <v>137</v>
       </c>
       <c r="C20" s="48" t="s">
-        <v>175</v>
+        <v>138</v>
       </c>
       <c r="D20" s="41" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E20" s="38" t="s">
         <v>51</v>
@@ -4065,25 +4062,25 @@
     </row>
     <row r="3" ht="109.5" customHeight="1">
       <c r="A3" s="30" t="s">
+        <v>209</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="C3" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="D3" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="F3" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="38" t="s">
         <v>214</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>215</v>
       </c>
       <c r="H3" s="43"/>
       <c r="I3" s="30"/>
@@ -4092,25 +4089,25 @@
     </row>
     <row r="4">
       <c r="A4" s="66" t="s">
+        <v>215</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="C4" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="C4" s="41" t="s">
+      <c r="D4" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E4" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="E4" s="41" t="s">
+      <c r="F4" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="41" t="s">
         <v>218</v>
-      </c>
-      <c r="F4" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="41" t="s">
-        <v>219</v>
       </c>
       <c r="H4" s="43"/>
       <c r="I4" s="43"/>
@@ -4119,25 +4116,25 @@
     </row>
     <row r="5">
       <c r="A5" s="66" t="s">
+        <v>219</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="C5" s="41" t="s">
         <v>220</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="C5" s="41" t="s">
+      <c r="D5" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E5" s="38" t="s">
         <v>221</v>
       </c>
-      <c r="D5" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="E5" s="38" t="s">
+      <c r="F5" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="38" t="s">
         <v>222</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="38" t="s">
-        <v>223</v>
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="43"/>
@@ -4146,25 +4143,25 @@
     </row>
     <row r="6">
       <c r="A6" s="66" t="s">
+        <v>223</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>224</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="38" t="s">
         <v>225</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="38" t="s">
         <v>226</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="F6" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="38" t="s">
         <v>227</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="38" t="s">
-        <v>228</v>
       </c>
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
@@ -4173,25 +4170,25 @@
     </row>
     <row r="7">
       <c r="A7" s="67" t="s">
+        <v>228</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="B7" s="58" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" s="59" t="s">
+      <c r="D7" s="60" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="D7" s="60" t="s">
-        <v>213</v>
-      </c>
-      <c r="E7" s="60" t="s">
+      <c r="F7" s="58" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="60" t="s">
         <v>231</v>
-      </c>
-      <c r="F7" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="60" t="s">
-        <v>232</v>
       </c>
       <c r="H7" s="61"/>
       <c r="I7" s="61"/>
@@ -4200,25 +4197,25 @@
     </row>
     <row r="8">
       <c r="A8" s="66" t="s">
+        <v>232</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="C8" s="41" t="s">
         <v>233</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="C8" s="41" t="s">
+      <c r="D8" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E8" s="41" t="s">
         <v>234</v>
       </c>
-      <c r="D8" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="E8" s="41" t="s">
+      <c r="F8" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="41" t="s">
         <v>235</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="41" t="s">
-        <v>236</v>
       </c>
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
@@ -4227,25 +4224,25 @@
     </row>
     <row r="9">
       <c r="A9" s="66" t="s">
+        <v>236</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="C9" s="41" t="s">
         <v>237</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" s="41" t="s">
+      <c r="D9" s="38" t="s">
+        <v>212</v>
+      </c>
+      <c r="E9" s="41" t="s">
         <v>238</v>
       </c>
-      <c r="D9" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="E9" s="41" t="s">
+      <c r="F9" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="41" t="s">
         <v>239</v>
-      </c>
-      <c r="F9" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="41" t="s">
-        <v>240</v>
       </c>
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
@@ -4363,25 +4360,25 @@
     </row>
     <row r="3" ht="243.0" customHeight="1">
       <c r="A3" s="30" t="s">
+        <v>240</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>241</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="C3" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="D3" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="38" t="s">
         <v>244</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="F3" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="38" t="s">
         <v>245</v>
-      </c>
-      <c r="F3" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="38" t="s">
-        <v>246</v>
       </c>
       <c r="H3" s="43"/>
       <c r="I3" s="30"/>
@@ -4390,25 +4387,25 @@
     </row>
     <row r="4">
       <c r="A4" s="68" t="s">
+        <v>246</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>241</v>
+      </c>
+      <c r="C4" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="B4" s="69" t="s">
-        <v>242</v>
-      </c>
-      <c r="C4" s="70" t="s">
+      <c r="D4" s="71" t="s">
+        <v>243</v>
+      </c>
+      <c r="E4" s="71" t="s">
         <v>248</v>
       </c>
-      <c r="D4" s="71" t="s">
-        <v>244</v>
-      </c>
-      <c r="E4" s="71" t="s">
+      <c r="F4" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="71" t="s">
         <v>249</v>
-      </c>
-      <c r="F4" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="71" t="s">
-        <v>250</v>
       </c>
       <c r="H4" s="72"/>
       <c r="I4" s="72"/>
@@ -4417,25 +4414,25 @@
     </row>
     <row r="5" ht="64.5" customHeight="1">
       <c r="A5" s="30" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C5" s="41" t="s">
         <v>251</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C5" s="41" t="s">
+      <c r="D5" s="41" t="s">
         <v>252</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="E5" s="38" t="s">
         <v>253</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="F5" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="41" t="s">
         <v>254</v>
-      </c>
-      <c r="F5" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="41" t="s">
-        <v>255</v>
       </c>
       <c r="H5" s="43"/>
       <c r="I5" s="43"/>
@@ -4444,25 +4441,25 @@
     </row>
     <row r="6">
       <c r="A6" s="30" t="s">
+        <v>255</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C6" s="41" t="s">
         <v>256</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C6" s="41" t="s">
+      <c r="D6" s="38" t="s">
         <v>257</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="38" t="s">
         <v>258</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="F6" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="41" t="s">
         <v>259</v>
-      </c>
-      <c r="F6" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="41" t="s">
-        <v>260</v>
       </c>
       <c r="H6" s="43"/>
       <c r="I6" s="43"/>
@@ -4471,25 +4468,25 @@
     </row>
     <row r="7">
       <c r="A7" s="30" t="s">
+        <v>260</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" s="41" t="s">
         <v>261</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C7" s="41" t="s">
+      <c r="D7" s="38" t="s">
         <v>262</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="E7" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="F7" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="38" t="s">
         <v>264</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="38" t="s">
-        <v>265</v>
       </c>
       <c r="H7" s="43"/>
       <c r="I7" s="43"/>
@@ -4498,25 +4495,25 @@
     </row>
     <row r="8">
       <c r="A8" s="30" t="s">
+        <v>265</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C8" s="41" t="s">
         <v>266</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C8" s="41" t="s">
+      <c r="D8" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E8" s="38" t="s">
+        <v>253</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="38" t="s">
         <v>267</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>263</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>254</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="38" t="s">
-        <v>268</v>
       </c>
       <c r="H8" s="43"/>
       <c r="I8" s="43"/>
@@ -4525,25 +4522,25 @@
     </row>
     <row r="9">
       <c r="A9" s="30" t="s">
+        <v>268</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>269</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C9" s="38" t="s">
+      <c r="D9" s="38" t="s">
+        <v>243</v>
+      </c>
+      <c r="E9" s="38" t="s">
         <v>270</v>
       </c>
-      <c r="D9" s="38" t="s">
-        <v>244</v>
-      </c>
-      <c r="E9" s="38" t="s">
+      <c r="F9" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="38" t="s">
         <v>271</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="38" t="s">
-        <v>272</v>
       </c>
       <c r="H9" s="43"/>
       <c r="I9" s="43"/>
@@ -4552,25 +4549,25 @@
     </row>
     <row r="10">
       <c r="A10" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>273</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C10" s="38" t="s">
+      <c r="D10" s="41" t="s">
         <v>274</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="E10" s="38" t="s">
         <v>275</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="F10" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G10" s="74" t="s">
         <v>276</v>
-      </c>
-      <c r="F10" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="74" t="s">
-        <v>277</v>
       </c>
       <c r="H10" s="43"/>
       <c r="I10" s="43"/>
@@ -4579,25 +4576,25 @@
     </row>
     <row r="11">
       <c r="A11" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C11" s="38" t="s">
         <v>278</v>
       </c>
-      <c r="B11" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C11" s="38" t="s">
+      <c r="D11" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="E11" s="38" t="s">
         <v>279</v>
       </c>
-      <c r="D11" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="E11" s="38" t="s">
+      <c r="F11" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="38" t="s">
         <v>280</v>
-      </c>
-      <c r="F11" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="38" t="s">
-        <v>281</v>
       </c>
       <c r="H11" s="43"/>
       <c r="I11" s="43"/>
@@ -4606,25 +4603,25 @@
     </row>
     <row r="12">
       <c r="A12" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C12" s="38" t="s">
         <v>282</v>
       </c>
-      <c r="B12" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C12" s="38" t="s">
+      <c r="D12" s="41" t="s">
+        <v>274</v>
+      </c>
+      <c r="E12" s="38" t="s">
         <v>283</v>
       </c>
-      <c r="D12" s="41" t="s">
-        <v>275</v>
-      </c>
-      <c r="E12" s="38" t="s">
+      <c r="F12" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" s="38" t="s">
         <v>284</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="38" t="s">
-        <v>285</v>
       </c>
       <c r="H12" s="43"/>
       <c r="I12" s="43"/>
@@ -4633,25 +4630,25 @@
     </row>
     <row r="13">
       <c r="A13" s="50" t="s">
+        <v>285</v>
+      </c>
+      <c r="B13" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="C13" s="60" t="s">
         <v>286</v>
       </c>
-      <c r="B13" s="58" t="s">
-        <v>242</v>
-      </c>
-      <c r="C13" s="60" t="s">
+      <c r="D13" s="59" t="s">
+        <v>274</v>
+      </c>
+      <c r="E13" s="59" t="s">
         <v>287</v>
       </c>
-      <c r="D13" s="59" t="s">
-        <v>275</v>
-      </c>
-      <c r="E13" s="59" t="s">
+      <c r="F13" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G13" s="59" t="s">
         <v>288</v>
-      </c>
-      <c r="F13" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="59" t="s">
-        <v>289</v>
       </c>
       <c r="H13" s="61"/>
       <c r="I13" s="61"/>
@@ -4660,25 +4657,25 @@
     </row>
     <row r="14">
       <c r="A14" s="30" t="s">
+        <v>289</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>290</v>
       </c>
-      <c r="B14" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C14" s="38" t="s">
+      <c r="D14" s="38" t="s">
+        <v>262</v>
+      </c>
+      <c r="E14" s="38" t="s">
         <v>291</v>
       </c>
-      <c r="D14" s="38" t="s">
-        <v>263</v>
-      </c>
-      <c r="E14" s="38" t="s">
+      <c r="F14" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="38" t="s">
         <v>292</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="38" t="s">
-        <v>293</v>
       </c>
       <c r="H14" s="43"/>
       <c r="I14" s="43"/>
@@ -4687,25 +4684,25 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="30" t="s">
+        <v>293</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>294</v>
       </c>
-      <c r="B15" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C15" s="38" t="s">
+      <c r="D15" s="38" t="s">
         <v>295</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="E15" s="38" t="s">
         <v>296</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="F15" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="38" t="s">
         <v>297</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>298</v>
       </c>
       <c r="H15" s="43"/>
       <c r="I15" s="43"/>
@@ -4714,25 +4711,25 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="50" t="s">
+        <v>298</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="C16" s="60" t="s">
         <v>299</v>
       </c>
-      <c r="B16" s="58" t="s">
-        <v>242</v>
-      </c>
-      <c r="C16" s="60" t="s">
+      <c r="D16" s="60" t="s">
+        <v>295</v>
+      </c>
+      <c r="E16" s="60" t="s">
         <v>300</v>
       </c>
-      <c r="D16" s="60" t="s">
-        <v>296</v>
-      </c>
-      <c r="E16" s="60" t="s">
+      <c r="F16" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="60" t="s">
         <v>301</v>
-      </c>
-      <c r="F16" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="60" t="s">
-        <v>302</v>
       </c>
       <c r="H16" s="61"/>
       <c r="I16" s="61"/>
@@ -4741,25 +4738,25 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="50" t="s">
+        <v>302</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>241</v>
+      </c>
+      <c r="C17" s="60" t="s">
         <v>303</v>
       </c>
-      <c r="B17" s="58" t="s">
-        <v>242</v>
-      </c>
-      <c r="C17" s="60" t="s">
+      <c r="D17" s="59" t="s">
+        <v>274</v>
+      </c>
+      <c r="E17" s="60" t="s">
         <v>304</v>
       </c>
-      <c r="D17" s="59" t="s">
-        <v>275</v>
-      </c>
-      <c r="E17" s="60" t="s">
+      <c r="F17" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="60" t="s">
         <v>305</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="60" t="s">
-        <v>306</v>
       </c>
       <c r="H17" s="61"/>
       <c r="I17" s="61"/>
@@ -4768,25 +4765,25 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="30" t="s">
+        <v>306</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" s="41" t="s">
         <v>307</v>
       </c>
-      <c r="B18" s="37" t="s">
-        <v>242</v>
-      </c>
-      <c r="C18" s="41" t="s">
+      <c r="D18" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="E18" s="41" t="s">
         <v>309</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="F18" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="41" t="s">
         <v>310</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="41" t="s">
-        <v>311</v>
       </c>
       <c r="H18" s="43"/>
       <c r="I18" s="43"/>
@@ -4907,25 +4904,25 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="77" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" s="37" t="s">
         <v>312</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="C3" s="42" t="s">
         <v>313</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="D3" s="38" t="s">
         <v>314</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="42" t="s">
         <v>315</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="F3" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G3" s="42" t="s">
         <v>316</v>
-      </c>
-      <c r="F3" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>317</v>
       </c>
       <c r="H3" s="78"/>
       <c r="I3" s="78"/>
@@ -4934,25 +4931,25 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="79" t="s">
+        <v>317</v>
+      </c>
+      <c r="B4" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>318</v>
       </c>
-      <c r="B4" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C4" s="42" t="s">
+      <c r="D4" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E4" s="42" t="s">
         <v>319</v>
       </c>
-      <c r="D4" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E4" s="42" t="s">
+      <c r="F4" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G4" s="42" t="s">
         <v>320</v>
-      </c>
-      <c r="F4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="42" t="s">
-        <v>321</v>
       </c>
       <c r="H4" s="78"/>
       <c r="I4" s="78"/>
@@ -4961,25 +4958,25 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="80" t="s">
+        <v>321</v>
+      </c>
+      <c r="B5" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" s="42" t="s">
         <v>322</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C5" s="42" t="s">
+      <c r="D5" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E5" s="42" t="s">
         <v>323</v>
       </c>
-      <c r="D5" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E5" s="42" t="s">
+      <c r="F5" s="66" t="s">
         <v>324</v>
       </c>
-      <c r="F5" s="66" t="s">
-        <v>325</v>
-      </c>
       <c r="G5" s="42" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="H5" s="78"/>
       <c r="I5" s="78"/>
@@ -4988,25 +4985,25 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="79" t="s">
+        <v>325</v>
+      </c>
+      <c r="B6" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C6" s="42" t="s">
         <v>326</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C6" s="42" t="s">
+      <c r="D6" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E6" s="42" t="s">
         <v>327</v>
       </c>
-      <c r="D6" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E6" s="42" t="s">
+      <c r="F6" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G6" s="42" t="s">
         <v>328</v>
-      </c>
-      <c r="F6" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="42" t="s">
-        <v>329</v>
       </c>
       <c r="H6" s="78"/>
       <c r="I6" s="78"/>
@@ -5015,25 +5012,25 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="80" t="s">
+        <v>329</v>
+      </c>
+      <c r="B7" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C7" s="42" t="s">
         <v>330</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C7" s="42" t="s">
+      <c r="D7" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E7" s="42" t="s">
         <v>331</v>
       </c>
-      <c r="D7" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>332</v>
-      </c>
       <c r="F7" s="30" t="s">
         <v>53</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H7" s="78"/>
       <c r="I7" s="78"/>
@@ -5042,25 +5039,25 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="80" t="s">
+        <v>332</v>
+      </c>
+      <c r="B8" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C8" s="42" t="s">
         <v>333</v>
       </c>
-      <c r="B8" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C8" s="42" t="s">
-        <v>334</v>
-      </c>
       <c r="D8" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E8" s="42" t="s">
         <v>315</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="F8" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="42" t="s">
         <v>316</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="42" t="s">
-        <v>317</v>
       </c>
       <c r="H8" s="78"/>
       <c r="I8" s="78"/>
@@ -5069,25 +5066,25 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="79" t="s">
+        <v>334</v>
+      </c>
+      <c r="B9" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C9" s="42" t="s">
         <v>335</v>
       </c>
-      <c r="B9" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C9" s="42" t="s">
+      <c r="D9" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E9" s="42" t="s">
         <v>336</v>
       </c>
-      <c r="D9" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E9" s="42" t="s">
-        <v>337</v>
-      </c>
       <c r="F9" s="30" t="s">
         <v>53</v>
       </c>
       <c r="G9" s="42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H9" s="78"/>
       <c r="I9" s="78"/>
@@ -5096,25 +5093,25 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="80" t="s">
+        <v>337</v>
+      </c>
+      <c r="B10" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C10" s="42" t="s">
         <v>338</v>
       </c>
-      <c r="B10" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C10" s="42" t="s">
+      <c r="D10" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E10" s="42" t="s">
         <v>339</v>
       </c>
-      <c r="D10" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E10" s="42" t="s">
-        <v>340</v>
-      </c>
       <c r="F10" s="30" t="s">
         <v>53</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="H10" s="78"/>
       <c r="I10" s="78"/>
@@ -5123,25 +5120,25 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="80" t="s">
+        <v>340</v>
+      </c>
+      <c r="B11" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C11" s="32" t="s">
         <v>341</v>
       </c>
-      <c r="B11" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C11" s="32" t="s">
+      <c r="D11" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E11" s="42" t="s">
         <v>342</v>
       </c>
-      <c r="D11" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E11" s="42" t="s">
+      <c r="F11" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="42" t="s">
         <v>343</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>344</v>
       </c>
       <c r="H11" s="78"/>
       <c r="I11" s="78"/>
@@ -5150,25 +5147,25 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="80" t="s">
+        <v>344</v>
+      </c>
+      <c r="B12" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C12" s="32" t="s">
         <v>345</v>
       </c>
-      <c r="B12" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C12" s="32" t="s">
+      <c r="D12" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E12" s="42" t="s">
         <v>346</v>
       </c>
-      <c r="D12" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E12" s="42" t="s">
-        <v>347</v>
-      </c>
       <c r="F12" s="30" t="s">
         <v>53</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H12" s="78"/>
       <c r="I12" s="78"/>
@@ -5177,25 +5174,25 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="79" t="s">
+        <v>347</v>
+      </c>
+      <c r="B13" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C13" s="42" t="s">
         <v>348</v>
       </c>
-      <c r="B13" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C13" s="42" t="s">
+      <c r="D13" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E13" s="42" t="s">
         <v>349</v>
       </c>
-      <c r="D13" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E13" s="42" t="s">
-        <v>350</v>
-      </c>
       <c r="F13" s="30" t="s">
         <v>53</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H13" s="78"/>
       <c r="I13" s="78"/>
@@ -5204,25 +5201,25 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="81" t="s">
+        <v>350</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C14" s="41" t="s">
         <v>351</v>
       </c>
-      <c r="B14" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C14" s="41" t="s">
+      <c r="D14" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E14" s="41" t="s">
         <v>352</v>
       </c>
-      <c r="D14" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E14" s="41" t="s">
+      <c r="F14" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G14" s="41" t="s">
         <v>353</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="41" t="s">
-        <v>354</v>
       </c>
       <c r="H14" s="43"/>
       <c r="I14" s="43"/>
@@ -5231,25 +5228,25 @@
     </row>
     <row r="15" ht="77.25" customHeight="1">
       <c r="A15" s="66" t="s">
+        <v>354</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>355</v>
       </c>
-      <c r="B15" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C15" s="38" t="s">
+      <c r="D15" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E15" s="38" t="s">
         <v>356</v>
       </c>
-      <c r="D15" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E15" s="38" t="s">
+      <c r="F15" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" s="38" t="s">
         <v>357</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="38" t="s">
-        <v>358</v>
       </c>
       <c r="H15" s="43"/>
       <c r="I15" s="43"/>
@@ -5258,25 +5255,25 @@
     </row>
     <row r="16" ht="48.0" customHeight="1">
       <c r="A16" s="66" t="s">
+        <v>358</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C16" s="41" t="s">
         <v>359</v>
       </c>
-      <c r="B16" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>360</v>
-      </c>
       <c r="D16" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E16" s="42" t="s">
         <v>315</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="F16" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="G16" s="42" t="s">
         <v>316</v>
-      </c>
-      <c r="F16" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="42" t="s">
-        <v>317</v>
       </c>
       <c r="H16" s="43"/>
       <c r="I16" s="43"/>
@@ -5285,25 +5282,25 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="82" t="s">
+        <v>360</v>
+      </c>
+      <c r="B17" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="C17" s="59" t="s">
         <v>361</v>
       </c>
-      <c r="B17" s="58" t="s">
-        <v>313</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>362</v>
-      </c>
       <c r="D17" s="60" t="s">
+        <v>314</v>
+      </c>
+      <c r="E17" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="E17" s="83" t="s">
+      <c r="F17" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G17" s="83" t="s">
         <v>316</v>
-      </c>
-      <c r="F17" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="83" t="s">
-        <v>317</v>
       </c>
       <c r="H17" s="61"/>
       <c r="I17" s="61"/>
@@ -5312,25 +5309,25 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="82" t="s">
+        <v>362</v>
+      </c>
+      <c r="B18" s="58" t="s">
+        <v>312</v>
+      </c>
+      <c r="C18" s="60" t="s">
         <v>363</v>
       </c>
-      <c r="B18" s="58" t="s">
-        <v>313</v>
-      </c>
-      <c r="C18" s="60" t="s">
-        <v>364</v>
-      </c>
       <c r="D18" s="60" t="s">
+        <v>314</v>
+      </c>
+      <c r="E18" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="E18" s="83" t="s">
+      <c r="F18" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="G18" s="83" t="s">
         <v>316</v>
-      </c>
-      <c r="F18" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="83" t="s">
-        <v>317</v>
       </c>
       <c r="H18" s="61"/>
       <c r="I18" s="61"/>
@@ -5339,25 +5336,25 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="66" t="s">
+        <v>364</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C19" s="38" t="s">
         <v>365</v>
       </c>
-      <c r="B19" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C19" s="38" t="s">
+      <c r="D19" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E19" s="42" t="s">
         <v>366</v>
       </c>
-      <c r="D19" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E19" s="42" t="s">
+      <c r="F19" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="42" t="s">
         <v>367</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>368</v>
       </c>
       <c r="H19" s="43"/>
       <c r="I19" s="43"/>
@@ -5366,25 +5363,25 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="66" t="s">
+        <v>368</v>
+      </c>
+      <c r="B20" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C20" s="38" t="s">
         <v>369</v>
       </c>
-      <c r="B20" s="37" t="s">
-        <v>313</v>
-      </c>
-      <c r="C20" s="38" t="s">
+      <c r="D20" s="38" t="s">
+        <v>314</v>
+      </c>
+      <c r="E20" s="42" t="s">
         <v>370</v>
       </c>
-      <c r="D20" s="38" t="s">
-        <v>315</v>
-      </c>
-      <c r="E20" s="42" t="s">
+      <c r="F20" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="42" t="s">
         <v>371</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="42" t="s">
-        <v>372</v>
       </c>
       <c r="H20" s="43"/>
       <c r="I20" s="43"/>

</xml_diff>

<commit_message>
MultiEnvironment Testing Setup finished. Docker and bat files added.
</commit_message>
<xml_diff>
--- a/Test Plan/Test Cases - in progress.xlsx
+++ b/Test Plan/Test Cases - in progress.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="681" uniqueCount="372">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="372">
   <si>
     <t>Project Name (Client Name)</t>
   </si>
@@ -134,6 +134,9 @@
   </si>
   <si>
     <t xml:space="preserve">Test Scenario </t>
+  </si>
+  <si>
+    <t>Automated</t>
   </si>
   <si>
     <t>Test Case Title</t>
@@ -168,6 +171,9 @@
   <si>
     <t>(TS_001) 
 Register Functionality</t>
+  </si>
+  <si>
+    <t>IN PROGRESS</t>
   </si>
   <si>
     <t>Validate Creating an Account by providing only the Mandatory fields</t>
@@ -645,9 +651,6 @@
     <t>Validate 'Create Account' functionality in all the supported environments</t>
   </si>
   <si>
-    <t>Automated</t>
-  </si>
-  <si>
     <t>TC_LF_001</t>
   </si>
   <si>
@@ -675,9 +678,6 @@
   <si>
     <t xml:space="preserve">"1.User should be taken to ""https://home.openweathermap.org/users/sign_in""
 2.User should be loggedin, username on menu and green successfully message at the top. </t>
-  </si>
-  <si>
-    <t>Pass</t>
   </si>
   <si>
     <t>TC_LF_002</t>
@@ -1640,10 +1640,20 @@
       <name val="Verdana"/>
     </font>
     <font>
+      <b/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
       <u/>
       <sz val="10.0"/>
       <color rgb="FF0563C1"/>
       <name val="Verdana"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -1666,20 +1676,10 @@
       <name val="Verdana"/>
     </font>
     <font>
-      <b/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Verdana"/>
-    </font>
-    <font>
       <u/>
       <sz val="10.0"/>
       <color theme="10"/>
       <name val="Verdana"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10.0"/>
@@ -1905,128 +1905,128 @@
     <xf borderId="2" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="7" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="2" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="7" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="2" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="18" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="2" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="15" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="7" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="2" fillId="4" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="6" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="20" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="2" fillId="3" fontId="17" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="4" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="7" fillId="3" fontId="18" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="4" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="3" fontId="19" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="20" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="15" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
     <xf borderId="0" fillId="3" fontId="21" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="5" fontId="14" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="5" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="5" fontId="16" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="5" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="2" fillId="4" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -2038,25 +2038,25 @@
     <xf borderId="7" fillId="3" fontId="23" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="4" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="4" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="2" fillId="3" fontId="16" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2672,15 +2672,16 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="21.43"/>
     <col customWidth="1" min="2" max="2" width="24.0"/>
-    <col customWidth="1" min="3" max="3" width="51.29"/>
-    <col customWidth="1" min="4" max="4" width="48.71"/>
-    <col customWidth="1" min="5" max="5" width="68.71"/>
-    <col customWidth="1" min="6" max="6" width="28.86"/>
-    <col customWidth="1" min="7" max="7" width="78.71"/>
-    <col customWidth="1" min="8" max="8" width="22.71"/>
-    <col customWidth="1" min="9" max="9" width="13.0"/>
-    <col customWidth="1" min="10" max="10" width="11.43"/>
-    <col customWidth="1" min="11" max="11" width="18.14"/>
+    <col customWidth="1" min="3" max="3" width="15.71"/>
+    <col customWidth="1" min="4" max="4" width="51.29"/>
+    <col customWidth="1" min="5" max="5" width="48.71"/>
+    <col customWidth="1" min="6" max="6" width="68.71"/>
+    <col customWidth="1" min="7" max="7" width="28.86"/>
+    <col customWidth="1" min="8" max="8" width="78.71"/>
+    <col customWidth="1" min="9" max="9" width="22.71"/>
+    <col customWidth="1" min="10" max="10" width="13.0"/>
+    <col customWidth="1" min="11" max="11" width="11.43"/>
+    <col customWidth="1" min="12" max="12" width="18.14"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2690,7 +2691,7 @@
       <c r="B1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="27" t="s">
@@ -2709,623 +2710,693 @@
         <v>44</v>
       </c>
       <c r="I1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="27" t="s">
         <v>21</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>45</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>46</v>
       </c>
+      <c r="L1" s="27" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="28" t="s">
-        <v>47</v>
+      <c r="A2" s="29" t="s">
+        <v>48</v>
       </c>
       <c r="B2" s="15"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" ht="160.5" customHeight="1">
-      <c r="A3" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="31" t="s">
+      <c r="A3" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="D3" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E3" s="32" t="s">
+      <c r="C3" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="33" t="s">
+      <c r="E3" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="F3" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H3" s="34"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="34"/>
+      <c r="G3" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" s="37"/>
+      <c r="J3" s="36"/>
+      <c r="K3" s="36"/>
+      <c r="L3" s="37"/>
     </row>
     <row r="4" ht="201.75" customHeight="1">
-      <c r="A4" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="B4" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="32" t="s">
+      <c r="A4" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="35" t="s">
+        <v>60</v>
+      </c>
+      <c r="I4" s="37"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="37"/>
+    </row>
+    <row r="5" ht="203.25" customHeight="1">
+      <c r="A5" s="32" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="D4" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E4" s="32" t="s">
-        <v>57</v>
-      </c>
-      <c r="F4" s="33" t="s">
+      <c r="I5" s="37"/>
+      <c r="J5" s="37"/>
+      <c r="K5" s="36"/>
+      <c r="L5" s="37"/>
+    </row>
+    <row r="6" ht="141.0" customHeight="1">
+      <c r="A6" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="B6" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="G4" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="H4" s="34"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="34"/>
-    </row>
-    <row r="5" ht="203.25" customHeight="1">
-      <c r="A5" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="F5" s="33" t="s">
+      <c r="F6" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="G6" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="I6" s="37"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="36"/>
+      <c r="L6" s="37"/>
+    </row>
+    <row r="7" ht="12.75" customHeight="1">
+      <c r="A7" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>69</v>
+      </c>
+      <c r="E7" s="35" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="F7" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="37"/>
+      <c r="J7" s="37"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="37"/>
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="35" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="I8" s="37"/>
+      <c r="J8" s="37"/>
+      <c r="K8" s="36"/>
+      <c r="L8" s="37"/>
+    </row>
+    <row r="9" ht="12.75" customHeight="1">
+      <c r="A9" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="36"/>
+      <c r="L9" s="37"/>
+    </row>
+    <row r="10" ht="12.75" customHeight="1">
+      <c r="A10" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>82</v>
+      </c>
+      <c r="G10" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="I10" s="37"/>
+      <c r="J10" s="37"/>
+      <c r="K10" s="36"/>
+      <c r="L10" s="37"/>
+    </row>
+    <row r="11" ht="12.75" customHeight="1">
+      <c r="A11" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="I11" s="37"/>
+      <c r="J11" s="37"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="37"/>
+    </row>
+    <row r="12" ht="12.75" customHeight="1">
+      <c r="A12" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="E12" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="38" t="s">
+        <v>92</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="37"/>
+      <c r="J12" s="37"/>
+      <c r="K12" s="36"/>
+      <c r="L12" s="37"/>
+    </row>
+    <row r="13" ht="12.75" customHeight="1">
+      <c r="A13" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="E13" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="H13" s="39" t="s">
+        <v>98</v>
+      </c>
+      <c r="I13" s="37"/>
+      <c r="J13" s="37"/>
+      <c r="K13" s="36"/>
+      <c r="L13" s="37"/>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" s="32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="I14" s="42"/>
+      <c r="J14" s="42"/>
+      <c r="K14" s="43"/>
+      <c r="L14" s="42"/>
+    </row>
+    <row r="15" ht="12.75" customHeight="1">
+      <c r="A15" s="32" t="s">
+        <v>103</v>
+      </c>
+      <c r="B15" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>104</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="G15" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="43"/>
+      <c r="L15" s="42"/>
+    </row>
+    <row r="16" ht="12.75" customHeight="1">
+      <c r="A16" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="B16" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>108</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="G16" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="42"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="43"/>
+      <c r="L16" s="42"/>
+    </row>
+    <row r="17" ht="12.75" customHeight="1">
+      <c r="A17" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="B17" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>112</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F17" s="35" t="s">
+        <v>113</v>
+      </c>
+      <c r="G17" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" s="42"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="43"/>
+      <c r="L17" s="42"/>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="G18" s="40">
+        <v>12345.0</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="43"/>
+      <c r="L18" s="42"/>
+    </row>
+    <row r="19" ht="12.75" customHeight="1">
+      <c r="A19" s="32" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F19" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="G19" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="35" t="s">
+        <v>122</v>
+      </c>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="42"/>
+    </row>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="41" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="41" t="s">
+        <v>126</v>
+      </c>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="46"/>
+    </row>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" s="32" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F21" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="46"/>
+    </row>
+    <row r="22" ht="12.75" customHeight="1">
+      <c r="A22" s="32" t="s">
+        <v>131</v>
+      </c>
+      <c r="B22" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>132</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="41" t="s">
+        <v>133</v>
+      </c>
+      <c r="G22" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="41" t="s">
+        <v>134</v>
+      </c>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="46"/>
+    </row>
+    <row r="23" ht="12.75" customHeight="1">
+      <c r="A23" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="B23" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>136</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F23" s="35" t="s">
         <v>54</v>
       </c>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="34"/>
-    </row>
-    <row r="6" ht="141.0" customHeight="1">
-      <c r="A6" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="B6" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="F6" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="32" t="s">
-        <v>65</v>
-      </c>
-      <c r="H6" s="34"/>
-      <c r="I6" s="34"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="34"/>
-    </row>
-    <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="30" t="s">
-        <v>66</v>
-      </c>
-      <c r="B7" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>68</v>
-      </c>
-      <c r="F7" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>69</v>
-      </c>
-      <c r="H7" s="34"/>
-      <c r="I7" s="34"/>
-      <c r="J7" s="33"/>
-      <c r="K7" s="34"/>
-    </row>
-    <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="30" t="s">
-        <v>70</v>
-      </c>
-      <c r="B8" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>72</v>
-      </c>
-      <c r="F8" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>73</v>
-      </c>
-      <c r="H8" s="34"/>
-      <c r="I8" s="34"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="34"/>
-    </row>
-    <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>75</v>
-      </c>
-      <c r="D9" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="F9" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>77</v>
-      </c>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="34"/>
-    </row>
-    <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="B10" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>79</v>
-      </c>
-      <c r="D10" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="F10" s="33" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>81</v>
-      </c>
-      <c r="H10" s="34"/>
-      <c r="I10" s="34"/>
-      <c r="J10" s="33"/>
-      <c r="K10" s="34"/>
-    </row>
-    <row r="11" ht="12.75" customHeight="1">
-      <c r="A11" s="30" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>83</v>
-      </c>
-      <c r="D11" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="34"/>
-      <c r="I11" s="34"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="34"/>
-    </row>
-    <row r="12" ht="12.75" customHeight="1">
-      <c r="A12" s="30" t="s">
-        <v>87</v>
-      </c>
-      <c r="B12" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>88</v>
-      </c>
-      <c r="D12" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="32" t="s">
-        <v>89</v>
-      </c>
-      <c r="F12" s="35" t="s">
-        <v>90</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="H12" s="34"/>
-      <c r="I12" s="34"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="34"/>
-    </row>
-    <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="30" t="s">
-        <v>92</v>
-      </c>
-      <c r="B13" s="31" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="35" t="s">
-        <v>95</v>
-      </c>
-      <c r="G13" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="H13" s="34"/>
-      <c r="I13" s="34"/>
-      <c r="J13" s="33"/>
-      <c r="K13" s="34"/>
-    </row>
-    <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="B14" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="32" t="s">
-        <v>99</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="40"/>
-      <c r="K14" s="39"/>
-    </row>
-    <row r="15" ht="12.75" customHeight="1">
-      <c r="A15" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>102</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>104</v>
-      </c>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="40"/>
-      <c r="K15" s="39"/>
-    </row>
-    <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>106</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E16" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>108</v>
-      </c>
-      <c r="H16" s="39"/>
-      <c r="I16" s="39"/>
-      <c r="J16" s="40"/>
-      <c r="K16" s="39"/>
-    </row>
-    <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="30" t="s">
-        <v>109</v>
-      </c>
-      <c r="B17" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>110</v>
-      </c>
-      <c r="D17" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E17" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="H17" s="39"/>
-      <c r="I17" s="39"/>
-      <c r="J17" s="40"/>
-      <c r="K17" s="39"/>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="B18" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>115</v>
-      </c>
-      <c r="F18" s="37">
-        <v>12345.0</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>116</v>
-      </c>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="40"/>
-      <c r="K18" s="39"/>
-    </row>
-    <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="B19" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>118</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E19" s="38" t="s">
-        <v>119</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>120</v>
-      </c>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="40"/>
-      <c r="K19" s="39"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="30" t="s">
-        <v>121</v>
-      </c>
-      <c r="B20" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>122</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>123</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="38" t="s">
-        <v>124</v>
-      </c>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="43"/>
-    </row>
-    <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="30" t="s">
-        <v>125</v>
-      </c>
-      <c r="B21" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" s="38" t="s">
-        <v>126</v>
-      </c>
-      <c r="D21" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="38" t="s">
-        <v>127</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G21" s="38" t="s">
-        <v>128</v>
-      </c>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="44"/>
-      <c r="K21" s="43"/>
-    </row>
-    <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="30" t="s">
-        <v>129</v>
-      </c>
-      <c r="B22" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E22" s="38" t="s">
-        <v>131</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="38" t="s">
-        <v>132</v>
-      </c>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="44"/>
-      <c r="K22" s="43"/>
-    </row>
-    <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="B23" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="C23" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="D23" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>53</v>
-      </c>
       <c r="G23" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="44"/>
-      <c r="K23" s="43"/>
+        <v>55</v>
+      </c>
+      <c r="H23" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="47"/>
+      <c r="L23" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J3:J23">
+  <conditionalFormatting sqref="K3:K23">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NOT TESTED">
-      <formula>NOT(ISERROR(SEARCH(("NOT TESTED"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("NOT TESTED"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J23">
+  <conditionalFormatting sqref="K3:K23">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="BLOCKED">
-      <formula>NOT(ISERROR(SEARCH(("BLOCKED"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("BLOCKED"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J23">
+  <conditionalFormatting sqref="K3:K23">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH(("FAIL"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("FAIL"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J23">
+  <conditionalFormatting sqref="K3:K23">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH(("PASS"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("PASS"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J3:J23">
+    <dataValidation type="list" allowBlank="1" sqref="C3:C23">
+      <formula1>"IN PROGRESS,YES,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K3:K23">
       <formula1>"PASS,FAIL,Blocked,Not Tested"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3367,359 +3438,357 @@
       <c r="B1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="45" t="s">
-        <v>135</v>
+      <c r="C1" s="28" t="s">
+        <v>39</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="F1" s="27" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G1" s="27" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H1" s="27" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I1" s="27" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J1" s="27" t="s">
         <v>21</v>
       </c>
       <c r="K1" s="27" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="L1" s="27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" ht="18.0" customHeight="1">
-      <c r="A2" s="46"/>
+      <c r="A2" s="48"/>
       <c r="B2" s="15"/>
-      <c r="C2" s="47"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
-      <c r="L2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" ht="18.0" customHeight="1">
-      <c r="A3" s="30" t="s">
-        <v>136</v>
-      </c>
-      <c r="B3" s="37" t="s">
+      <c r="A3" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D3" s="41" t="s">
+      <c r="C3" s="34" t="s">
         <v>139</v>
       </c>
-      <c r="E3" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="32" t="s">
+      <c r="D3" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="E3" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F3" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="G3" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="I3" s="43"/>
-      <c r="J3" s="30"/>
-      <c r="K3" s="49" t="s">
+      <c r="H3" s="41" t="s">
         <v>143</v>
       </c>
-      <c r="L3" s="43"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="46"/>
     </row>
     <row r="4" ht="18.0" customHeight="1">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="32" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C4" s="48" t="s">
+      <c r="B4" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="C4" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D4" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="E4" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F4" s="32" t="s">
+      <c r="E4" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F4" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="G4" s="37" t="s">
+      <c r="G4" s="40" t="s">
         <v>147</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="44"/>
-      <c r="L4" s="43"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="46"/>
     </row>
     <row r="5" ht="18.0" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="B5" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5" s="48" t="s">
+      <c r="B5" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="C5" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D5" s="44" t="s">
         <v>150</v>
       </c>
-      <c r="E5" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F5" s="32" t="s">
+      <c r="E5" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="G5" s="32" t="s">
+      <c r="G5" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="H5" s="38" t="s">
+      <c r="H5" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="43"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="46"/>
     </row>
     <row r="6" ht="18.0" customHeight="1">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="32" t="s">
         <v>152</v>
       </c>
-      <c r="B6" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="48" t="s">
+      <c r="B6" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="C6" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D6" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="E6" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="32" t="s">
+      <c r="E6" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="G6" s="32" t="s">
+      <c r="G6" s="35" t="s">
         <v>154</v>
       </c>
-      <c r="H6" s="38" t="s">
+      <c r="H6" s="41" t="s">
         <v>148</v>
       </c>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="44"/>
-      <c r="L6" s="43"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="46"/>
     </row>
     <row r="7" ht="18.0" customHeight="1">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="32" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C7" s="48" t="s">
+      <c r="B7" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="C7" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D7" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="32" t="s">
+      <c r="E7" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="35" t="s">
         <v>157</v>
       </c>
-      <c r="G7" s="30" t="s">
+      <c r="G7" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>148</v>
+      </c>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="46"/>
+    </row>
+    <row r="8" ht="18.0" customHeight="1">
+      <c r="A8" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>159</v>
+      </c>
+      <c r="E8" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="H7" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="43"/>
-    </row>
-    <row r="8" ht="18.0" customHeight="1">
-      <c r="A8" s="30" t="s">
-        <v>158</v>
-      </c>
-      <c r="B8" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" s="48" t="s">
+      <c r="F8" s="35" t="s">
+        <v>160</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="46"/>
+    </row>
+    <row r="9" ht="18.0" customHeight="1">
+      <c r="A9" s="32" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D8" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>160</v>
-      </c>
-      <c r="G8" s="30" t="s">
+      <c r="C9" s="34" t="s">
+        <v>163</v>
+      </c>
+      <c r="D9" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="E9" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="H8" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="44"/>
-      <c r="L8" s="43"/>
-    </row>
-    <row r="9" ht="18.0" customHeight="1">
-      <c r="A9" s="30" t="s">
-        <v>162</v>
-      </c>
-      <c r="B9" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" s="48" t="s">
+      <c r="F9" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="G9" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="H9" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="46"/>
+    </row>
+    <row r="10" ht="18.0" customHeight="1">
+      <c r="A10" s="32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B10" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="44" t="s">
+        <v>167</v>
+      </c>
+      <c r="E10" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="G10" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="41" t="s">
+        <v>169</v>
+      </c>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="46"/>
+    </row>
+    <row r="11" ht="18.0" customHeight="1">
+      <c r="A11" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="B11" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F11" s="35" t="s">
+        <v>172</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>142</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="46"/>
+    </row>
+    <row r="12" ht="18.0" customHeight="1">
+      <c r="A12" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="B12" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D9" s="41" t="s">
-        <v>164</v>
-      </c>
-      <c r="E9" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F9" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="G9" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="H9" s="38" t="s">
+      <c r="D12" s="44" t="s">
+        <v>175</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F12" s="35" t="s">
+        <v>176</v>
+      </c>
+      <c r="G12" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="43"/>
-    </row>
-    <row r="10" ht="18.0" customHeight="1">
-      <c r="A10" s="30" t="s">
-        <v>166</v>
-      </c>
-      <c r="B10" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C10" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>167</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="32" t="s">
-        <v>168</v>
-      </c>
-      <c r="G10" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="H10" s="38" t="s">
-        <v>169</v>
-      </c>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="44"/>
-      <c r="L10" s="43"/>
-    </row>
-    <row r="11" ht="18.0" customHeight="1">
-      <c r="A11" s="30" t="s">
-        <v>170</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="48" t="s">
-        <v>138</v>
-      </c>
-      <c r="D11" s="41" t="s">
-        <v>171</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="38" t="s">
-        <v>173</v>
-      </c>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
-      <c r="K11" s="44"/>
-      <c r="L11" s="43"/>
-    </row>
-    <row r="12" ht="18.0" customHeight="1">
-      <c r="A12" s="30" t="s">
-        <v>174</v>
-      </c>
-      <c r="B12" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C12" s="48" t="s">
-        <v>163</v>
-      </c>
-      <c r="D12" s="41" t="s">
-        <v>175</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>141</v>
-      </c>
-      <c r="H12" s="38" t="s">
+      <c r="H12" s="41" t="s">
         <v>177</v>
       </c>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
-      <c r="K12" s="44"/>
-      <c r="L12" s="43"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13" ht="18.0" customHeight="1">
       <c r="A13" s="50" t="s">
         <v>178</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C13" s="52" t="s">
         <v>163</v>
@@ -3728,12 +3797,12 @@
         <v>179</v>
       </c>
       <c r="E13" s="54" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F13" s="55"/>
       <c r="G13" s="55"/>
       <c r="H13" s="54" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="I13" s="56"/>
       <c r="J13" s="56"/>
@@ -3741,71 +3810,71 @@
       <c r="L13" s="56"/>
     </row>
     <row r="14" ht="18.0" customHeight="1">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="32" t="s">
         <v>180</v>
       </c>
-      <c r="B14" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C14" s="48" t="s">
+      <c r="B14" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="E14" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="32" t="s">
+      <c r="E14" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="G14" s="32" t="s">
+      <c r="G14" s="35" t="s">
         <v>183</v>
       </c>
-      <c r="H14" s="38" t="s">
+      <c r="H14" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="44"/>
-      <c r="L14" s="43"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="46"/>
     </row>
     <row r="15" ht="18.0" customHeight="1">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="32" t="s">
         <v>185</v>
       </c>
-      <c r="B15" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C15" s="48" t="s">
+      <c r="B15" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="C15" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D15" s="44" t="s">
         <v>186</v>
       </c>
-      <c r="E15" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="32" t="s">
+      <c r="E15" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F15" s="35" t="s">
         <v>187</v>
       </c>
-      <c r="G15" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="H15" s="38" t="s">
+      <c r="G15" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="41" t="s">
         <v>188</v>
       </c>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="44"/>
-      <c r="L15" s="43"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="46"/>
     </row>
     <row r="16" ht="18.0" customHeight="1">
       <c r="A16" s="50" t="s">
         <v>189</v>
       </c>
       <c r="B16" s="58" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C16" s="52" t="s">
         <v>163</v>
@@ -3814,7 +3883,7 @@
         <v>190</v>
       </c>
       <c r="E16" s="60" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F16" s="54" t="s">
         <v>191</v>
@@ -3835,7 +3904,7 @@
         <v>194</v>
       </c>
       <c r="B17" s="58" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C17" s="52" t="s">
         <v>163</v>
@@ -3844,7 +3913,7 @@
         <v>195</v>
       </c>
       <c r="E17" s="60" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F17" s="64" t="s">
         <v>196</v>
@@ -3861,39 +3930,39 @@
       <c r="L17" s="61"/>
     </row>
     <row r="18" ht="18.0" customHeight="1">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="B18" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C18" s="48" t="s">
+      <c r="B18" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="C18" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D18" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="E18" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F18" s="32" t="s">
+      <c r="E18" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F18" s="35" t="s">
         <v>201</v>
       </c>
-      <c r="G18" s="30"/>
-      <c r="H18" s="38" t="s">
+      <c r="G18" s="32"/>
+      <c r="H18" s="41" t="s">
         <v>202</v>
       </c>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="44"/>
-      <c r="L18" s="43"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="46"/>
     </row>
     <row r="19" ht="18.0" customHeight="1">
       <c r="A19" s="50" t="s">
         <v>203</v>
       </c>
       <c r="B19" s="58" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="C19" s="52" t="s">
         <v>163</v>
@@ -3902,13 +3971,13 @@
         <v>204</v>
       </c>
       <c r="E19" s="60" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F19" s="54" t="s">
         <v>205</v>
       </c>
       <c r="G19" s="50" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="H19" s="59" t="s">
         <v>206</v>
@@ -3919,34 +3988,34 @@
       <c r="L19" s="61"/>
     </row>
     <row r="20" ht="18.0" customHeight="1">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="B20" s="37" t="s">
-        <v>137</v>
-      </c>
-      <c r="C20" s="48" t="s">
+      <c r="B20" s="40" t="s">
         <v>138</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="C20" s="34" t="s">
+        <v>139</v>
+      </c>
+      <c r="D20" s="44" t="s">
         <v>208</v>
       </c>
-      <c r="E20" s="38" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G20" s="32" t="s">
+      <c r="E20" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="H20" s="38" t="s">
+      <c r="G20" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="44"/>
-      <c r="L20" s="43"/>
+      <c r="H20" s="41" t="s">
+        <v>143</v>
+      </c>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3999,15 +4068,16 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="15.14"/>
     <col customWidth="1" min="2" max="2" width="21.29"/>
-    <col customWidth="1" min="3" max="3" width="28.86"/>
-    <col customWidth="1" min="4" max="4" width="33.43"/>
-    <col customWidth="1" min="5" max="5" width="49.0"/>
-    <col customWidth="1" min="6" max="6" width="31.71"/>
-    <col customWidth="1" min="7" max="7" width="45.71"/>
-    <col customWidth="1" min="8" max="8" width="29.43"/>
-    <col customWidth="1" min="9" max="9" width="13.0"/>
-    <col customWidth="1" min="10" max="10" width="10.57"/>
-    <col customWidth="1" min="11" max="11" width="22.57"/>
+    <col customWidth="1" min="3" max="3" width="15.71"/>
+    <col customWidth="1" min="4" max="4" width="28.86"/>
+    <col customWidth="1" min="5" max="5" width="33.43"/>
+    <col customWidth="1" min="6" max="6" width="49.0"/>
+    <col customWidth="1" min="7" max="7" width="31.71"/>
+    <col customWidth="1" min="8" max="8" width="45.71"/>
+    <col customWidth="1" min="9" max="9" width="29.43"/>
+    <col customWidth="1" min="10" max="10" width="13.0"/>
+    <col customWidth="1" min="11" max="11" width="10.57"/>
+    <col customWidth="1" min="12" max="12" width="22.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4017,7 +4087,7 @@
       <c r="B1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="27" t="s">
@@ -4036,137 +4106,153 @@
         <v>44</v>
       </c>
       <c r="I1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="27" t="s">
         <v>21</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>45</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>46</v>
       </c>
+      <c r="L1" s="27" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="46" t="s">
-        <v>47</v>
+      <c r="A2" s="48" t="s">
+        <v>48</v>
       </c>
       <c r="B2" s="15"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" ht="109.5" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="32" t="s">
         <v>209</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="C3" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="F3" s="41" t="s">
         <v>213</v>
       </c>
-      <c r="F3" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="49"/>
-      <c r="K3" s="43"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="46"/>
     </row>
     <row r="4">
       <c r="A4" s="66" t="s">
         <v>215</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="E4" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="F4" s="44" t="s">
         <v>217</v>
       </c>
-      <c r="F4" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="44" t="s">
         <v>218</v>
       </c>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="43"/>
+      <c r="I4" s="46"/>
+      <c r="J4" s="46"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="46"/>
     </row>
     <row r="5">
       <c r="A5" s="66" t="s">
         <v>219</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="44" t="s">
         <v>220</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="E5" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="F5" s="41" t="s">
         <v>221</v>
       </c>
-      <c r="F5" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="38" t="s">
+      <c r="G5" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="43"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="46"/>
     </row>
     <row r="6">
       <c r="A6" s="66" t="s">
         <v>223</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="F6" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="F6" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="38" t="s">
+      <c r="G6" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="41" t="s">
         <v>227</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="43"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="46"/>
     </row>
     <row r="7">
       <c r="A7" s="67" t="s">
@@ -4175,107 +4261,119 @@
       <c r="B7" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="C7" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="59" t="s">
         <v>229</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="E7" s="60" t="s">
         <v>212</v>
       </c>
-      <c r="E7" s="60" t="s">
+      <c r="F7" s="60" t="s">
         <v>230</v>
       </c>
-      <c r="F7" s="58" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="60" t="s">
+      <c r="G7" s="58" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="60" t="s">
         <v>231</v>
       </c>
-      <c r="H7" s="61"/>
       <c r="I7" s="61"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="61"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="61"/>
     </row>
     <row r="8">
       <c r="A8" s="66" t="s">
         <v>232</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="44" t="s">
         <v>233</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="E8" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="F8" s="44" t="s">
         <v>234</v>
       </c>
-      <c r="F8" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="41" t="s">
+      <c r="G8" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="44" t="s">
         <v>235</v>
       </c>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="43"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="46"/>
     </row>
     <row r="9">
       <c r="A9" s="66" t="s">
         <v>236</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="40" t="s">
         <v>210</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="E9" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="F9" s="44" t="s">
         <v>238</v>
       </c>
-      <c r="F9" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="41" t="s">
+      <c r="G9" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="43"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J3:J9">
+  <conditionalFormatting sqref="K3:K9">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NOT TESTED">
-      <formula>NOT(ISERROR(SEARCH(("NOT TESTED"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("NOT TESTED"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J9">
+  <conditionalFormatting sqref="K3:K9">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="BLOCKED">
-      <formula>NOT(ISERROR(SEARCH(("BLOCKED"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("BLOCKED"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J9">
+  <conditionalFormatting sqref="K3:K9">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH(("FAIL"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("FAIL"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J9">
+  <conditionalFormatting sqref="K3:K9">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH(("PASS"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("PASS"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J3:J9">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K3:K9">
       <formula1>"PASS,FAIL,Blocked,Not Tested"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="C3:C9">
+      <formula1>"IN PROGRESS,YES,NO"</formula1>
     </dataValidation>
   </dataValidations>
   <printOptions/>
@@ -4297,15 +4395,16 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="11.57"/>
     <col customWidth="1" min="2" max="2" width="21.29"/>
-    <col customWidth="1" min="3" max="3" width="28.86"/>
-    <col customWidth="1" min="4" max="4" width="33.43"/>
-    <col customWidth="1" min="5" max="5" width="49.0"/>
-    <col customWidth="1" min="6" max="6" width="31.71"/>
-    <col customWidth="1" min="7" max="7" width="45.71"/>
-    <col customWidth="1" min="8" max="8" width="29.43"/>
-    <col customWidth="1" min="9" max="9" width="13.0"/>
-    <col customWidth="1" min="10" max="10" width="10.57"/>
-    <col customWidth="1" min="11" max="11" width="22.57"/>
+    <col customWidth="1" min="3" max="3" width="15.71"/>
+    <col customWidth="1" min="4" max="4" width="28.86"/>
+    <col customWidth="1" min="5" max="5" width="33.43"/>
+    <col customWidth="1" min="6" max="6" width="49.0"/>
+    <col customWidth="1" min="7" max="7" width="31.71"/>
+    <col customWidth="1" min="8" max="8" width="45.71"/>
+    <col customWidth="1" min="9" max="9" width="29.43"/>
+    <col customWidth="1" min="10" max="10" width="13.0"/>
+    <col customWidth="1" min="11" max="11" width="10.57"/>
+    <col customWidth="1" min="12" max="12" width="22.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4315,7 +4414,7 @@
       <c r="B1" s="27" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="27" t="s">
@@ -4334,56 +4433,63 @@
         <v>44</v>
       </c>
       <c r="I1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="27" t="s">
         <v>21</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>45</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>46</v>
       </c>
+      <c r="L1" s="27" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="46" t="s">
-        <v>47</v>
+      <c r="A2" s="48" t="s">
+        <v>48</v>
       </c>
       <c r="B2" s="15"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" ht="243.0" customHeight="1">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="44" t="s">
         <v>242</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="41" t="s">
         <v>243</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="F3" s="41" t="s">
         <v>244</v>
       </c>
-      <c r="F3" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="38" t="s">
+      <c r="G3" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="H3" s="43"/>
-      <c r="I3" s="30"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="43"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="46"/>
     </row>
     <row r="4">
       <c r="A4" s="68" t="s">
@@ -4392,241 +4498,268 @@
       <c r="B4" s="69" t="s">
         <v>241</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="70" t="s">
         <v>247</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="E4" s="71" t="s">
         <v>243</v>
       </c>
-      <c r="E4" s="71" t="s">
+      <c r="F4" s="71" t="s">
         <v>248</v>
       </c>
-      <c r="F4" s="69" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="71" t="s">
         <v>249</v>
       </c>
-      <c r="H4" s="72"/>
       <c r="I4" s="72"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="73"/>
+      <c r="L4" s="72"/>
     </row>
     <row r="5" ht="64.5" customHeight="1">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="44" t="s">
         <v>251</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="E5" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="E5" s="38" t="s">
+      <c r="F5" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="F5" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="44" t="s">
         <v>254</v>
       </c>
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="43"/>
+      <c r="I5" s="46"/>
+      <c r="J5" s="46"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="46"/>
     </row>
     <row r="6">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="32" t="s">
         <v>255</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="44" t="s">
         <v>256</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="41" t="s">
         <v>257</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="F6" s="41" t="s">
         <v>258</v>
       </c>
-      <c r="F6" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="44" t="s">
         <v>259</v>
       </c>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="43"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="46"/>
     </row>
     <row r="7">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="32" t="s">
         <v>260</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="44" t="s">
         <v>261</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="E7" s="41" t="s">
         <v>262</v>
       </c>
-      <c r="E7" s="38" t="s">
+      <c r="F7" s="41" t="s">
         <v>263</v>
       </c>
-      <c r="F7" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="38" t="s">
+      <c r="G7" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="41" t="s">
         <v>264</v>
       </c>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="43"/>
+      <c r="I7" s="46"/>
+      <c r="J7" s="46"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="46"/>
     </row>
     <row r="8">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="32" t="s">
         <v>265</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="44" t="s">
         <v>266</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="E8" s="41" t="s">
         <v>262</v>
       </c>
-      <c r="E8" s="38" t="s">
+      <c r="F8" s="41" t="s">
         <v>253</v>
       </c>
-      <c r="F8" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="38" t="s">
+      <c r="G8" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="41" t="s">
         <v>267</v>
       </c>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="43"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="46"/>
     </row>
     <row r="9">
-      <c r="A9" s="30" t="s">
+      <c r="A9" s="32" t="s">
         <v>268</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="C9" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="41" t="s">
         <v>269</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="E9" s="41" t="s">
         <v>243</v>
       </c>
-      <c r="E9" s="38" t="s">
+      <c r="F9" s="41" t="s">
         <v>270</v>
       </c>
-      <c r="F9" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="38" t="s">
+      <c r="G9" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="43"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="46"/>
     </row>
     <row r="10">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="32" t="s">
         <v>272</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="C10" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="41" t="s">
         <v>273</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="E10" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="E10" s="38" t="s">
+      <c r="F10" s="41" t="s">
         <v>275</v>
       </c>
-      <c r="F10" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="74" t="s">
+      <c r="G10" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="74" t="s">
         <v>276</v>
       </c>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="43"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="46"/>
     </row>
     <row r="11">
-      <c r="A11" s="30" t="s">
+      <c r="A11" s="32" t="s">
         <v>277</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="C11" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="41" t="s">
         <v>278</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="E11" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="E11" s="38" t="s">
+      <c r="F11" s="41" t="s">
         <v>279</v>
       </c>
-      <c r="F11" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="38" t="s">
+      <c r="G11" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="43"/>
+      <c r="I11" s="46"/>
+      <c r="J11" s="46"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="46"/>
     </row>
     <row r="12">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="32" t="s">
         <v>281</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="C12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="41" t="s">
         <v>282</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="E12" s="44" t="s">
         <v>274</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="F12" s="41" t="s">
         <v>283</v>
       </c>
-      <c r="F12" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="38" t="s">
+      <c r="G12" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="41" t="s">
         <v>284</v>
       </c>
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="43"/>
+      <c r="I12" s="46"/>
+      <c r="J12" s="46"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="46"/>
     </row>
     <row r="13">
       <c r="A13" s="50" t="s">
@@ -4635,79 +4768,88 @@
       <c r="B13" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="60" t="s">
         <v>286</v>
       </c>
-      <c r="D13" s="59" t="s">
+      <c r="E13" s="59" t="s">
         <v>274</v>
       </c>
-      <c r="E13" s="59" t="s">
+      <c r="F13" s="59" t="s">
         <v>287</v>
       </c>
-      <c r="F13" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="59" t="s">
+      <c r="G13" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="59" t="s">
         <v>288</v>
       </c>
-      <c r="H13" s="61"/>
       <c r="I13" s="61"/>
-      <c r="J13" s="62"/>
-      <c r="K13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="61"/>
     </row>
     <row r="14">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="32" t="s">
         <v>289</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="C14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="41" t="s">
         <v>290</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="E14" s="41" t="s">
         <v>262</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="F14" s="41" t="s">
         <v>291</v>
       </c>
-      <c r="F14" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="43"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="46"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="32" t="s">
         <v>293</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="41" t="s">
         <v>294</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="E15" s="41" t="s">
         <v>295</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="F15" s="41" t="s">
         <v>296</v>
       </c>
-      <c r="F15" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="41" t="s">
         <v>297</v>
       </c>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="43"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="46"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="50" t="s">
@@ -4716,25 +4858,28 @@
       <c r="B16" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="C16" s="60" t="s">
+      <c r="C16" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="60" t="s">
         <v>299</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="E16" s="60" t="s">
         <v>295</v>
       </c>
-      <c r="E16" s="60" t="s">
+      <c r="F16" s="60" t="s">
         <v>300</v>
       </c>
-      <c r="F16" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="60" t="s">
+      <c r="G16" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="60" t="s">
         <v>301</v>
       </c>
-      <c r="H16" s="61"/>
       <c r="I16" s="61"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="61"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="61"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="50" t="s">
@@ -4743,84 +4888,93 @@
       <c r="B17" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="60" t="s">
         <v>303</v>
       </c>
-      <c r="D17" s="59" t="s">
+      <c r="E17" s="59" t="s">
         <v>274</v>
       </c>
-      <c r="E17" s="60" t="s">
+      <c r="F17" s="60" t="s">
         <v>304</v>
       </c>
-      <c r="F17" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="60" t="s">
+      <c r="G17" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="60" t="s">
         <v>305</v>
       </c>
-      <c r="H17" s="61"/>
       <c r="I17" s="61"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="61"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="32" t="s">
         <v>306</v>
       </c>
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="40" t="s">
         <v>241</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="44" t="s">
         <v>307</v>
       </c>
-      <c r="D18" s="38" t="s">
+      <c r="E18" s="41" t="s">
         <v>308</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="F18" s="44" t="s">
         <v>309</v>
       </c>
-      <c r="F18" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="41" t="s">
+      <c r="G18" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="44" t="s">
         <v>310</v>
       </c>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="43"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="47"/>
+      <c r="L18" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J3:J18">
+  <conditionalFormatting sqref="K3:K18">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NOT TESTED">
-      <formula>NOT(ISERROR(SEARCH(("NOT TESTED"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("NOT TESTED"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J18">
+  <conditionalFormatting sqref="K3:K18">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="BLOCKED">
-      <formula>NOT(ISERROR(SEARCH(("BLOCKED"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("BLOCKED"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J18">
+  <conditionalFormatting sqref="K3:K18">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH(("FAIL"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("FAIL"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J18">
+  <conditionalFormatting sqref="K3:K18">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH(("PASS"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("PASS"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J3:J18">
+    <dataValidation type="list" allowBlank="1" sqref="C3:C18">
+      <formula1>"IN PROGRESS,YES,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K3:K18">
       <formula1>"PASS,FAIL,Blocked,Not Tested"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="G10"/>
+    <hyperlink r:id="rId1" ref="H10"/>
   </hyperlinks>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
@@ -4841,15 +4995,16 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="14.0"/>
     <col customWidth="1" min="2" max="2" width="21.29"/>
-    <col customWidth="1" min="3" max="3" width="28.86"/>
-    <col customWidth="1" min="4" max="4" width="33.43"/>
-    <col customWidth="1" min="5" max="5" width="56.29"/>
-    <col customWidth="1" min="6" max="6" width="31.71"/>
-    <col customWidth="1" min="7" max="7" width="45.71"/>
-    <col customWidth="1" min="8" max="8" width="29.43"/>
-    <col customWidth="1" min="9" max="9" width="13.0"/>
-    <col customWidth="1" min="10" max="10" width="14.0"/>
-    <col customWidth="1" min="11" max="11" width="22.57"/>
+    <col customWidth="1" min="3" max="3" width="15.71"/>
+    <col customWidth="1" min="4" max="4" width="28.86"/>
+    <col customWidth="1" min="5" max="5" width="33.43"/>
+    <col customWidth="1" min="6" max="6" width="56.29"/>
+    <col customWidth="1" min="7" max="7" width="31.71"/>
+    <col customWidth="1" min="8" max="8" width="45.71"/>
+    <col customWidth="1" min="9" max="9" width="29.43"/>
+    <col customWidth="1" min="10" max="10" width="13.0"/>
+    <col customWidth="1" min="11" max="11" width="14.0"/>
+    <col customWidth="1" min="12" max="12" width="22.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -4859,7 +5014,7 @@
       <c r="B1" s="75" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="28" t="s">
         <v>39</v>
       </c>
       <c r="D1" s="27" t="s">
@@ -4878,407 +5033,453 @@
         <v>44</v>
       </c>
       <c r="I1" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" s="27" t="s">
         <v>21</v>
-      </c>
-      <c r="J1" s="27" t="s">
-        <v>45</v>
       </c>
       <c r="K1" s="27" t="s">
         <v>46</v>
       </c>
+      <c r="L1" s="27" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="76" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B2" s="15"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="29"/>
-      <c r="K2" s="29"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="77" t="s">
         <v>311</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C3" s="42" t="s">
+      <c r="C3" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="45" t="s">
         <v>313</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="E3" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="F3" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="F3" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H3" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="H3" s="78"/>
       <c r="I3" s="78"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="78"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="47"/>
+      <c r="L3" s="78"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="79" t="s">
         <v>317</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="45" t="s">
         <v>318</v>
       </c>
-      <c r="D4" s="38" t="s">
+      <c r="E4" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="F4" s="45" t="s">
         <v>319</v>
       </c>
-      <c r="F4" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H4" s="45" t="s">
         <v>320</v>
       </c>
-      <c r="H4" s="78"/>
       <c r="I4" s="78"/>
-      <c r="J4" s="44"/>
-      <c r="K4" s="78"/>
+      <c r="J4" s="78"/>
+      <c r="K4" s="47"/>
+      <c r="L4" s="78"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="80" t="s">
         <v>321</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="45" t="s">
         <v>322</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="E5" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="F5" s="45" t="s">
         <v>323</v>
       </c>
-      <c r="F5" s="66" t="s">
+      <c r="G5" s="66" t="s">
         <v>324</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="H5" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="H5" s="78"/>
       <c r="I5" s="78"/>
-      <c r="J5" s="44"/>
-      <c r="K5" s="78"/>
+      <c r="J5" s="78"/>
+      <c r="K5" s="47"/>
+      <c r="L5" s="78"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="79" t="s">
         <v>325</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="45" t="s">
         <v>326</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="F6" s="45" t="s">
         <v>327</v>
       </c>
-      <c r="F6" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" s="45" t="s">
         <v>328</v>
       </c>
-      <c r="H6" s="78"/>
       <c r="I6" s="78"/>
-      <c r="J6" s="44"/>
-      <c r="K6" s="78"/>
+      <c r="J6" s="78"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="78"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="80" t="s">
         <v>329</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="45" t="s">
         <v>330</v>
       </c>
-      <c r="D7" s="38" t="s">
+      <c r="E7" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="F7" s="45" t="s">
         <v>331</v>
       </c>
-      <c r="F7" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="45" t="s">
         <v>320</v>
       </c>
-      <c r="H7" s="78"/>
       <c r="I7" s="78"/>
-      <c r="J7" s="44"/>
-      <c r="K7" s="78"/>
+      <c r="J7" s="78"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="78"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="80" t="s">
         <v>332</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="45" t="s">
         <v>333</v>
       </c>
-      <c r="D8" s="38" t="s">
+      <c r="E8" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E8" s="42" t="s">
+      <c r="F8" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="F8" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G8" s="42" t="s">
+      <c r="G8" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="H8" s="78"/>
       <c r="I8" s="78"/>
-      <c r="J8" s="44"/>
-      <c r="K8" s="78"/>
+      <c r="J8" s="78"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="78"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="79" t="s">
         <v>334</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C9" s="42" t="s">
+      <c r="C9" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="45" t="s">
         <v>335</v>
       </c>
-      <c r="D9" s="38" t="s">
+      <c r="E9" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E9" s="42" t="s">
+      <c r="F9" s="45" t="s">
         <v>336</v>
       </c>
-      <c r="F9" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G9" s="42" t="s">
+      <c r="G9" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H9" s="45" t="s">
         <v>320</v>
       </c>
-      <c r="H9" s="78"/>
       <c r="I9" s="78"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="78"/>
+      <c r="J9" s="78"/>
+      <c r="K9" s="47"/>
+      <c r="L9" s="78"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="80" t="s">
         <v>337</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="45" t="s">
         <v>338</v>
       </c>
-      <c r="D10" s="38" t="s">
+      <c r="E10" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E10" s="42" t="s">
+      <c r="F10" s="45" t="s">
         <v>339</v>
       </c>
-      <c r="F10" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G10" s="42" t="s">
+      <c r="G10" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="45" t="s">
         <v>320</v>
       </c>
-      <c r="H10" s="78"/>
       <c r="I10" s="78"/>
-      <c r="J10" s="44"/>
-      <c r="K10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="47"/>
+      <c r="L10" s="78"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="80" t="s">
         <v>340</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="35" t="s">
         <v>341</v>
       </c>
-      <c r="D11" s="38" t="s">
+      <c r="E11" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E11" s="42" t="s">
+      <c r="F11" s="45" t="s">
         <v>342</v>
       </c>
-      <c r="F11" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="42" t="s">
+      <c r="G11" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="45" t="s">
         <v>343</v>
       </c>
-      <c r="H11" s="78"/>
       <c r="I11" s="78"/>
-      <c r="J11" s="44"/>
-      <c r="K11" s="78"/>
+      <c r="J11" s="78"/>
+      <c r="K11" s="47"/>
+      <c r="L11" s="78"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="80" t="s">
         <v>344</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="35" t="s">
         <v>345</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="E12" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E12" s="42" t="s">
+      <c r="F12" s="45" t="s">
         <v>346</v>
       </c>
-      <c r="F12" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G12" s="42" t="s">
+      <c r="G12" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H12" s="45" t="s">
         <v>343</v>
       </c>
-      <c r="H12" s="78"/>
       <c r="I12" s="78"/>
-      <c r="J12" s="44"/>
-      <c r="K12" s="78"/>
+      <c r="J12" s="78"/>
+      <c r="K12" s="47"/>
+      <c r="L12" s="78"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="79" t="s">
         <v>347</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C13" s="42" t="s">
+      <c r="C13" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="45" t="s">
         <v>348</v>
       </c>
-      <c r="D13" s="38" t="s">
+      <c r="E13" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="F13" s="45" t="s">
         <v>349</v>
       </c>
-      <c r="F13" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H13" s="45" t="s">
         <v>343</v>
       </c>
-      <c r="H13" s="78"/>
       <c r="I13" s="78"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="78"/>
+      <c r="J13" s="78"/>
+      <c r="K13" s="47"/>
+      <c r="L13" s="78"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="81" t="s">
         <v>350</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="44" t="s">
         <v>351</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="E14" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="F14" s="44" t="s">
         <v>352</v>
       </c>
-      <c r="F14" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G14" s="41" t="s">
+      <c r="G14" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H14" s="44" t="s">
         <v>353</v>
       </c>
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="44"/>
-      <c r="K14" s="43"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="47"/>
+      <c r="L14" s="46"/>
     </row>
     <row r="15" ht="77.25" customHeight="1">
       <c r="A15" s="66" t="s">
         <v>354</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="C15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D15" s="41" t="s">
         <v>355</v>
       </c>
-      <c r="D15" s="38" t="s">
+      <c r="E15" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="F15" s="41" t="s">
         <v>356</v>
       </c>
-      <c r="F15" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G15" s="38" t="s">
+      <c r="G15" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H15" s="41" t="s">
         <v>357</v>
       </c>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="44"/>
-      <c r="K15" s="43"/>
+      <c r="I15" s="46"/>
+      <c r="J15" s="46"/>
+      <c r="K15" s="47"/>
+      <c r="L15" s="46"/>
     </row>
     <row r="16" ht="48.0" customHeight="1">
       <c r="A16" s="66" t="s">
         <v>358</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D16" s="44" t="s">
         <v>359</v>
       </c>
-      <c r="D16" s="38" t="s">
+      <c r="E16" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="F16" s="45" t="s">
         <v>315</v>
       </c>
-      <c r="F16" s="37" t="s">
-        <v>53</v>
-      </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="44"/>
-      <c r="K16" s="43"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="47"/>
+      <c r="L16" s="46"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="82" t="s">
@@ -5287,25 +5488,28 @@
       <c r="B17" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="59" t="s">
         <v>361</v>
       </c>
-      <c r="D17" s="60" t="s">
+      <c r="E17" s="60" t="s">
         <v>314</v>
       </c>
-      <c r="E17" s="83" t="s">
+      <c r="F17" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="F17" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G17" s="83" t="s">
+      <c r="G17" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="H17" s="83" t="s">
         <v>316</v>
       </c>
-      <c r="H17" s="61"/>
       <c r="I17" s="61"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="61"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="61"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="82" t="s">
@@ -5314,106 +5518,118 @@
       <c r="B18" s="58" t="s">
         <v>312</v>
       </c>
-      <c r="C18" s="60" t="s">
+      <c r="C18" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="60" t="s">
         <v>363</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="E18" s="60" t="s">
         <v>314</v>
       </c>
-      <c r="E18" s="83" t="s">
+      <c r="F18" s="83" t="s">
         <v>315</v>
       </c>
-      <c r="F18" s="50" t="s">
-        <v>53</v>
-      </c>
-      <c r="G18" s="83" t="s">
+      <c r="G18" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="H18" s="83" t="s">
         <v>316</v>
       </c>
-      <c r="H18" s="61"/>
       <c r="I18" s="61"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="61"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="61"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="66" t="s">
         <v>364</v>
       </c>
-      <c r="B19" s="37" t="s">
+      <c r="B19" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="C19" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="41" t="s">
         <v>365</v>
       </c>
-      <c r="D19" s="38" t="s">
+      <c r="E19" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="F19" s="45" t="s">
         <v>366</v>
       </c>
-      <c r="F19" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" s="45" t="s">
         <v>367</v>
       </c>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="43"/>
+      <c r="I19" s="46"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="46"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="66" t="s">
         <v>368</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="40" t="s">
         <v>312</v>
       </c>
-      <c r="C20" s="38" t="s">
+      <c r="C20" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="41" t="s">
         <v>369</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="E20" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="F20" s="45" t="s">
         <v>370</v>
       </c>
-      <c r="F20" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="G20" s="42" t="s">
+      <c r="G20" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="45" t="s">
         <v>371</v>
       </c>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="44"/>
-      <c r="K20" s="43"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="47"/>
+      <c r="L20" s="46"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:B2"/>
   </mergeCells>
-  <conditionalFormatting sqref="J3:J20">
+  <conditionalFormatting sqref="K3:K20">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="NOT TESTED">
-      <formula>NOT(ISERROR(SEARCH(("NOT TESTED"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("NOT TESTED"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J20">
+  <conditionalFormatting sqref="K3:K20">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="BLOCKED">
-      <formula>NOT(ISERROR(SEARCH(("BLOCKED"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("BLOCKED"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J20">
+  <conditionalFormatting sqref="K3:K20">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH(("FAIL"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("FAIL"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J3:J20">
+  <conditionalFormatting sqref="K3:K20">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="PASS">
-      <formula>NOT(ISERROR(SEARCH(("PASS"),(J3))))</formula>
+      <formula>NOT(ISERROR(SEARCH(("PASS"),(K3))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="J3:J20">
+    <dataValidation type="list" allowBlank="1" sqref="C3:C20">
+      <formula1>"IN PROGRESS,YES,NO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="K3:K20">
       <formula1>"PASS,FAIL,Blocked,Not Tested"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>